<commit_message>
Aggiornata checklist per casi 45,48,51
Aggiornata checklist per casi 45,48,51 (coerenza tra campi da P a R con quanto indicato in colonna S)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
@@ -497,7 +497,7 @@
     <t xml:space="preserve">Il servizio FSE non è attualmente disponibile, non è possibile validare e pubblicare il referto sul Fascicolo Elettronico del paziente al momento. Verrà tentato in automatico di pubblicarlo in un momento successivo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene segnalato al medico che il servizio di FSE per validare il referto non è raggiungibile. Viene consentito di consegnare il referto al paziente. Un processo in background ritenterà l'invio in un momento successivo; nel caso in cui il CDA non risultasse valido, non verrà alimentato il FSE con questo referto.</t>
+    <t xml:space="preserve">Viene segnalato al medico che il servizio di FSE per validare il referto non è raggiungibile. Viene consentito di consegnare il referto al paziente. Un processo in background ritenterà l'invio in un momento successivo.</t>
   </si>
   <si>
     <t>VALIDAZIONE_PSS_TIMEOUT</t>
@@ -5312,10 +5312,10 @@
         <v>61</v>
       </c>
       <c r="Q28" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="R28" s="49" t="s">
         <v>61</v>
-      </c>
-      <c r="R28" s="49" t="s">
-        <v>60</v>
       </c>
       <c r="S28" s="50" t="s">
         <v>100</v>
@@ -5447,10 +5447,10 @@
         <v>61</v>
       </c>
       <c r="Q31" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="R31" s="49" t="s">
         <v>61</v>
-      </c>
-      <c r="R31" s="49" t="s">
-        <v>60</v>
       </c>
       <c r="S31" s="50" t="s">
         <v>100</v>
@@ -5582,10 +5582,10 @@
         <v>61</v>
       </c>
       <c r="Q34" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="R34" s="49" t="s">
         <v>61</v>
-      </c>
-      <c r="R34" s="49" t="s">
-        <v>60</v>
       </c>
       <c r="S34" s="50" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Rifatti test per tipologie già accreditate
Aggiornati data.json e report-checklist con gli esiti dei test per le tipologia LDO, VPS e RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
@@ -358,10 +358,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:29:33Z</t>
-  </si>
-  <si>
-    <t>dd8affc82e434027cbf1204ca13a467a</t>
+    <t>2025-11-14T14:40:59Z</t>
+  </si>
+  <si>
+    <t>2c1188de654be2a4c3b565bdc18b9463</t>
   </si>
   <si>
     <t>PSS</t>
@@ -388,10 +388,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:26:18Z</t>
-  </si>
-  <si>
-    <t>42386932ae83157a8ae19ccf8b362ae5</t>
+    <t>2025-11-14T14:45:04Z</t>
+  </si>
+  <si>
+    <t>9b2d9c119b11bb9dfd3fc4176a5fe14f</t>
   </si>
   <si>
     <t>CERT_VAC</t>
@@ -412,10 +412,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:28:02Z</t>
-  </si>
-  <si>
-    <t>c44216a04b95ccef8ef0669d5b2e15ad</t>
+    <t>2025-11-14T14:46:39Z</t>
+  </si>
+  <si>
+    <t>190239189ec22cacbc2ebedd432bab69</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
@@ -472,10 +472,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:31:03Z</t>
-  </si>
-  <si>
-    <t>44a675a1dc4c5a08e3f2d3ef5dd68c68</t>
+    <t>2025-11-14T14:56:18Z</t>
+  </si>
+  <si>
+    <t>e007a22273b9ac83fe16fc502ff26e17</t>
   </si>
   <si>
     <t xml:space="preserve">Si è verificato un errore durante la comunicazione con FSE. Dettaglio Errore: "Campo token JWT non valido. - Il campo action_id non è corretto". Contattare il CED.</t>
@@ -496,10 +496,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:32:30Z</t>
-  </si>
-  <si>
-    <t>17ef7ee8fedf3900124c8cf445931eb4</t>
+    <t>2025-11-14T14:57:18Z</t>
+  </si>
+  <si>
+    <t>bf6f16d460ffa8e07a06d28cacfe7ce6</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -511,10 +511,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_VPS_KO</t>
   </si>
   <si>
-    <t>2025-09-18T07:33:16Z</t>
-  </si>
-  <si>
-    <t>59e0842c730f8bda83089c0aaa87d16f</t>
+    <t>2025-11-14T14:58:09Z</t>
+  </si>
+  <si>
+    <t>4799f8707bef94e09aba0245aba025f4</t>
   </si>
   <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
@@ -1536,13 +1536,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:26:36Z</t>
-  </si>
-  <si>
-    <t>cff9156076d2cc7e3a56578a9c8263bd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.d0f3005de28a3be0d00e357ee2f4708b0f6e7b663b9260f495f5249f54234f8a.674d593d84^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T14:59:45Z</t>
+  </si>
+  <si>
+    <t>86ff9eb37c297cb77a264303c217da60</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.d0f3005de28a3be0d00e357ee2f4708b0f6e7b663b9260f495f5249f54234f8a.682cabbc03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT25</t>
@@ -1552,13 +1552,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:28:06Z</t>
-  </si>
-  <si>
-    <t>a8115008446649f7cf63a92ecb1c7829</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.d0f3005de28a3be0d00e357ee2f4708b0f6e7b663b9260f495f5249f54234f8a.1bddb7dbe1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T15:02:18Z</t>
+  </si>
+  <si>
+    <t>8354354791156a3502f9217cb0fac0ea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.d0f3005de28a3be0d00e357ee2f4708b0f6e7b663b9260f495f5249f54234f8a.e08c1f8198^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT17</t>
@@ -1568,13 +1568,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:29:46Z</t>
-  </si>
-  <si>
-    <t>0e8ee1e0edefd8e3486c810b44334dbc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.2170324c8e63caac57df0df20f4086940f467875b189fefe016d1b3144cf74b8.9196587ade^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T15:03:54Z</t>
+  </si>
+  <si>
+    <t>a8982d869b71846553eb9d78ce003250</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.2170324c8e63caac57df0df20f4086940f467875b189fefe016d1b3144cf74b8.fffcc4f0e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT18</t>
@@ -1584,13 +1584,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 18" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:31:55Z</t>
-  </si>
-  <si>
-    <t>13294b9c711c7fa34857b228776e4483</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.2170324c8e63caac57df0df20f4086940f467875b189fefe016d1b3144cf74b8.e419e6712e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T15:04:57Z</t>
+  </si>
+  <si>
+    <t>aa51e5543f944f592493505397ebbd2f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.2170324c8e63caac57df0df20f4086940f467875b189fefe016d1b3144cf74b8.6728e29953^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT17</t>
@@ -1617,13 +1617,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 30" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:33:06Z</t>
-  </si>
-  <si>
-    <t>9cb2b227d92d3021fa020d49c7475825</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.6d3954027e89b57178211a527fe93b27519999f3acd6c3b753748443ada6ebd4.117d30c9d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T15:06:06Z</t>
+  </si>
+  <si>
+    <t>d7eda121e0ee8f25d09c7c531a55c96a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.6d3954027e89b57178211a527fe93b27519999f3acd6c3b753748443ada6ebd4.c7644bd7e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT31</t>
@@ -1633,13 +1633,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 31" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-09-19T15:34:04Z</t>
-  </si>
-  <si>
-    <t>30965be35cb7a4d372d255db92de534f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.6d3954027e89b57178211a527fe93b27519999f3acd6c3b753748443ada6ebd4.f415fd2326^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-11-14T15:07:24Z</t>
+  </si>
+  <si>
+    <t>6884b12d63bc05c8ebe2a804ab3ce241</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.160.4.5.160080.6d3954027e89b57178211a527fe93b27519999f3acd6c3b753748443ada6ebd4.3825eaf19a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_SING_VAC_CT4</t>
@@ -2006,7 +2006,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2390,17 +2390,6 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="none"/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -2420,7 +2409,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2568,13 +2557,10 @@
     <xf fontId="2" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="30" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="3" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="3" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="3" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="3" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="8" fillId="0" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2583,17 +2569,17 @@
     <xf fontId="9" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -4628,7 +4614,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" ht="128.25">
+    <row r="10" ht="128.25" hidden="1">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4675,7 +4661,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" ht="11" customHeight="1">
+    <row r="11" ht="11" hidden="1" customHeight="1">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -4736,7 +4722,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" ht="40.5" hidden="1" customHeight="1">
+    <row r="12" ht="40.5" customHeight="1">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -4753,7 +4739,7 @@
         <v>57</v>
       </c>
       <c r="F12" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G12" s="46" t="s">
         <v>67</v>
@@ -4834,7 +4820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" ht="11" customHeight="1">
+    <row r="14" ht="11" hidden="1" customHeight="1">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -4895,7 +4881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" ht="74.25" hidden="1" customHeight="1">
+    <row r="15" ht="74.25" customHeight="1">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -4912,7 +4898,7 @@
         <v>57</v>
       </c>
       <c r="F15" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G15" s="48" t="s">
         <v>77</v>
@@ -5030,7 +5016,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" ht="39" hidden="1" customHeight="1">
+    <row r="18" ht="39" customHeight="1">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -5047,7 +5033,7 @@
         <v>57</v>
       </c>
       <c r="F18" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G18" s="49" t="s">
         <v>85</v>
@@ -5091,7 +5077,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" ht="39" customHeight="1">
+    <row r="19" ht="39" hidden="1" customHeight="1">
       <c r="A19" s="35">
         <v>36</v>
       </c>
@@ -5152,7 +5138,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" ht="39" hidden="1" customHeight="1">
+    <row r="20" ht="39" customHeight="1">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -5169,7 +5155,7 @@
         <v>88</v>
       </c>
       <c r="F20" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G20" s="46" t="s">
         <v>92</v>
@@ -5250,7 +5236,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" ht="35.25" customHeight="1">
+    <row r="22" ht="35.25" hidden="1" customHeight="1">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -5311,7 +5297,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" ht="39" hidden="1" customHeight="1">
+    <row r="23" ht="39" customHeight="1">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -5328,7 +5314,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G23" s="44" t="s">
         <v>100</v>
@@ -5446,7 +5432,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" ht="39" hidden="1" customHeight="1">
+    <row r="26" ht="39" customHeight="1">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -5463,7 +5449,7 @@
         <v>88</v>
       </c>
       <c r="F26" s="43">
-        <v>45918</v>
+        <v>45975</v>
       </c>
       <c r="G26" s="44" t="s">
         <v>105</v>
@@ -5507,7 +5493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" ht="39" customHeight="1">
+    <row r="27" ht="39" hidden="1" customHeight="1">
       <c r="A27" s="35">
         <v>44</v>
       </c>
@@ -5660,7 +5646,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" ht="39" customHeight="1">
+    <row r="30" ht="39" hidden="1" customHeight="1">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -5909,7 +5895,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" ht="39" customHeight="1">
+    <row r="35" ht="39" hidden="1" customHeight="1">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5950,7 +5936,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" ht="39" customHeight="1">
+    <row r="36" ht="39" hidden="1" customHeight="1">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5991,7 +5977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" ht="39" customHeight="1">
+    <row r="37" ht="39" hidden="1" customHeight="1">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -6032,7 +6018,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" ht="39" customHeight="1">
+    <row r="38" ht="39" hidden="1" customHeight="1">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -6073,7 +6059,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" ht="39" customHeight="1">
+    <row r="39" ht="39" hidden="1" customHeight="1">
       <c r="A39" s="35">
         <v>59</v>
       </c>
@@ -6114,7 +6100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" ht="39" customHeight="1">
+    <row r="40" ht="39" hidden="1" customHeight="1">
       <c r="A40" s="35">
         <v>60</v>
       </c>
@@ -6155,7 +6141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" ht="39" customHeight="1">
+    <row r="41" ht="39" hidden="1" customHeight="1">
       <c r="A41" s="35">
         <v>61</v>
       </c>
@@ -6196,7 +6182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" ht="39" customHeight="1">
+    <row r="42" ht="39" hidden="1" customHeight="1">
       <c r="A42" s="35">
         <v>62</v>
       </c>
@@ -6647,7 +6633,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" ht="39" customHeight="1">
+    <row r="53" ht="39" hidden="1" customHeight="1">
       <c r="A53" s="35">
         <v>76</v>
       </c>
@@ -6688,7 +6674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" ht="39" customHeight="1">
+    <row r="54" ht="39" hidden="1" customHeight="1">
       <c r="A54" s="35">
         <v>78</v>
       </c>
@@ -6729,7 +6715,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" ht="39" customHeight="1">
+    <row r="55" ht="39" hidden="1" customHeight="1">
       <c r="A55" s="35">
         <v>79</v>
       </c>
@@ -6770,7 +6756,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" ht="39" customHeight="1">
+    <row r="56" ht="39" hidden="1" customHeight="1">
       <c r="A56" s="35">
         <v>80</v>
       </c>
@@ -6811,7 +6797,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" ht="39" customHeight="1">
+    <row r="57" ht="39" hidden="1" customHeight="1">
       <c r="A57" s="35">
         <v>81</v>
       </c>
@@ -6852,7 +6838,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" ht="39" customHeight="1">
+    <row r="58" ht="39" hidden="1" customHeight="1">
       <c r="A58" s="35">
         <v>83</v>
       </c>
@@ -6893,7 +6879,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" ht="39" customHeight="1">
+    <row r="59" ht="39" hidden="1" customHeight="1">
       <c r="A59" s="35">
         <v>84</v>
       </c>
@@ -6934,7 +6920,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" ht="39" customHeight="1">
+    <row r="60" ht="39" hidden="1" customHeight="1">
       <c r="A60" s="35">
         <v>85</v>
       </c>
@@ -6975,7 +6961,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" ht="39" customHeight="1">
+    <row r="61" ht="39" hidden="1" customHeight="1">
       <c r="A61" s="35">
         <v>86</v>
       </c>
@@ -7016,7 +7002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" ht="39" customHeight="1">
+    <row r="62" ht="39" hidden="1" customHeight="1">
       <c r="A62" s="35">
         <v>87</v>
       </c>
@@ -7057,7 +7043,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" ht="39" customHeight="1">
+    <row r="63" ht="39" hidden="1" customHeight="1">
       <c r="A63" s="35">
         <v>88</v>
       </c>
@@ -7098,7 +7084,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" ht="39" customHeight="1">
+    <row r="64" ht="39" hidden="1" customHeight="1">
       <c r="A64" s="35">
         <v>89</v>
       </c>
@@ -7139,7 +7125,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" ht="39" customHeight="1">
+    <row r="65" ht="39" hidden="1" customHeight="1">
       <c r="A65" s="35">
         <v>90</v>
       </c>
@@ -7180,7 +7166,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" ht="39" customHeight="1">
+    <row r="66" ht="39" hidden="1" customHeight="1">
       <c r="A66" s="35">
         <v>91</v>
       </c>
@@ -7221,7 +7207,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" ht="39" customHeight="1">
+    <row r="67" ht="39" hidden="1" customHeight="1">
       <c r="A67" s="35">
         <v>92</v>
       </c>
@@ -7262,7 +7248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" ht="39" customHeight="1">
+    <row r="68" ht="39" hidden="1" customHeight="1">
       <c r="A68" s="35">
         <v>93</v>
       </c>
@@ -10304,7 +10290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" ht="15">
+    <row r="146" ht="15" hidden="1">
       <c r="A146" s="35">
         <v>191</v>
       </c>
@@ -10351,7 +10337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="147" ht="39" customHeight="1">
+    <row r="147" ht="39" hidden="1" customHeight="1">
       <c r="A147" s="35">
         <v>376</v>
       </c>
@@ -10394,7 +10380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="148" ht="39" customHeight="1">
+    <row r="148" ht="39" hidden="1" customHeight="1">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -10441,7 +10427,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="149" ht="39" customHeight="1">
+    <row r="149" ht="39" hidden="1" customHeight="1">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -10488,7 +10474,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="150" ht="39" customHeight="1">
+    <row r="150" ht="39" hidden="1" customHeight="1">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -10535,7 +10521,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="151" ht="39" customHeight="1">
+    <row r="151" ht="39" hidden="1" customHeight="1">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -10596,7 +10582,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="152" ht="39" customHeight="1">
+    <row r="152" ht="39" hidden="1" customHeight="1">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -10657,7 +10643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="153" ht="39" customHeight="1">
+    <row r="153" ht="39" hidden="1" customHeight="1">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -10714,7 +10700,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="154" ht="39" customHeight="1">
+    <row r="154" ht="39" hidden="1" customHeight="1">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -10755,7 +10741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="155" ht="39" customHeight="1">
+    <row r="155" ht="39" hidden="1" customHeight="1">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -10796,7 +10782,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="156" ht="39" customHeight="1">
+    <row r="156" ht="39" hidden="1" customHeight="1">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -10837,7 +10823,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" ht="39" customHeight="1">
+    <row r="157" ht="39" hidden="1" customHeight="1">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -10878,7 +10864,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="158" ht="39" customHeight="1">
+    <row r="158" ht="39" hidden="1" customHeight="1">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -10919,7 +10905,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="159" ht="39" customHeight="1">
+    <row r="159" ht="39" hidden="1" customHeight="1">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -10960,7 +10946,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="160" ht="39" customHeight="1">
+    <row r="160" ht="39" hidden="1" customHeight="1">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -11001,7 +10987,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="161" ht="39" customHeight="1">
+    <row r="161" ht="39" hidden="1" customHeight="1">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -11042,7 +11028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="162" ht="39" customHeight="1">
+    <row r="162" ht="39" hidden="1" customHeight="1">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -11083,7 +11069,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" ht="39" customHeight="1">
+    <row r="163" ht="39" hidden="1" customHeight="1">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -11198,7 +11184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="166" ht="39" hidden="1" customHeight="1">
+    <row r="166" ht="39" customHeight="1">
       <c r="A166" s="35">
         <v>448</v>
       </c>
@@ -11214,10 +11200,10 @@
       <c r="E166" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="F166" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G166" s="38" t="s">
+      <c r="F166" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G166" s="49" t="s">
         <v>401</v>
       </c>
       <c r="H166" s="38" t="s">
@@ -11245,7 +11231,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="167" ht="33" hidden="1" customHeight="1">
+    <row r="167" ht="33" customHeight="1">
       <c r="A167" s="35">
         <v>449</v>
       </c>
@@ -11261,10 +11247,10 @@
       <c r="E167" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="F167" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G167" s="38" t="s">
+      <c r="F167" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G167" s="49" t="s">
         <v>406</v>
       </c>
       <c r="H167" s="38" t="s">
@@ -11292,7 +11278,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="168" ht="33.75" hidden="1" customHeight="1">
+    <row r="168" ht="33.75" customHeight="1">
       <c r="A168" s="35">
         <v>450</v>
       </c>
@@ -11308,10 +11294,10 @@
       <c r="E168" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="F168" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G168" s="57" t="s">
+      <c r="F168" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G168" s="49" t="s">
         <v>411</v>
       </c>
       <c r="H168" s="38" t="s">
@@ -11339,7 +11325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="169" ht="20.25" hidden="1" customHeight="1">
+    <row r="169" ht="20.25" customHeight="1">
       <c r="A169" s="35">
         <v>451</v>
       </c>
@@ -11355,10 +11341,10 @@
       <c r="E169" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="F169" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G169" s="45" t="s">
+      <c r="F169" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G169" s="44" t="s">
         <v>416</v>
       </c>
       <c r="H169" s="38" t="s">
@@ -11386,7 +11372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="170" ht="15">
+    <row r="170" ht="15" hidden="1">
       <c r="A170" s="35">
         <v>452</v>
       </c>
@@ -11405,7 +11391,7 @@
       <c r="F170" s="38">
         <v>45967</v>
       </c>
-      <c r="G170" s="38" t="s">
+      <c r="G170" s="47" t="s">
         <v>421</v>
       </c>
       <c r="H170" s="38" t="s">
@@ -11433,7 +11419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" ht="14.25" hidden="1" customHeight="1">
+    <row r="171" ht="14.25" customHeight="1">
       <c r="A171" s="35">
         <v>454</v>
       </c>
@@ -11449,10 +11435,10 @@
       <c r="E171" s="36" t="s">
         <v>425</v>
       </c>
-      <c r="F171" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G171" s="57" t="s">
+      <c r="F171" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G171" s="49" t="s">
         <v>426</v>
       </c>
       <c r="H171" s="38" t="s">
@@ -11480,7 +11466,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="172" ht="14.25" hidden="1" customHeight="1">
+    <row r="172" ht="14.25" customHeight="1">
       <c r="A172" s="35">
         <v>455</v>
       </c>
@@ -11496,10 +11482,10 @@
       <c r="E172" s="36" t="s">
         <v>430</v>
       </c>
-      <c r="F172" s="38">
-        <v>45919</v>
-      </c>
-      <c r="G172" s="38" t="s">
+      <c r="F172" s="43">
+        <v>45975</v>
+      </c>
+      <c r="G172" s="44" t="s">
         <v>431</v>
       </c>
       <c r="H172" s="38" t="s">
@@ -11675,7 +11661,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="177" ht="15">
+    <row r="177" ht="15" hidden="1">
       <c r="A177" s="35">
         <v>460</v>
       </c>
@@ -11763,7 +11749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="179" ht="15">
+    <row r="179" ht="15" hidden="1">
       <c r="A179" s="35">
         <v>462</v>
       </c>
@@ -11919,7 +11905,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" ht="15">
+    <row r="183" ht="15" hidden="1">
       <c r="A183" s="35">
         <v>466</v>
       </c>
@@ -12079,7 +12065,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="187" ht="15">
+    <row r="187" ht="15" hidden="1">
       <c r="A187" s="35">
         <v>470</v>
       </c>
@@ -12120,7 +12106,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="188" ht="15">
+    <row r="188" ht="15" hidden="1">
       <c r="A188" s="35">
         <v>471</v>
       </c>
@@ -12167,7 +12153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="189" ht="15">
+    <row r="189" ht="15" hidden="1">
       <c r="A189" s="35">
         <v>472</v>
       </c>
@@ -12214,7 +12200,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="190" ht="15">
+    <row r="190" ht="15" hidden="1">
       <c r="A190" s="35">
         <v>473</v>
       </c>
@@ -12255,7 +12241,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="191" ht="15">
+    <row r="191" ht="15" hidden="1">
       <c r="A191" s="35">
         <v>474</v>
       </c>
@@ -16357,10 +16343,15 @@
   <autoFilter ref="A9:W192">
     <filterColumn colId="2">
       <filters>
-        <filter val="LAB"/>
-        <filter val="RAD"/>
-        <filter val="RAP"/>
+        <filter val="LDO"/>
+        <filter val="RSA"/>
+        <filter val="VPS"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters and="1">
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="7">
@@ -16750,170 +16741,170 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="57" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="58" t="s">
         <v>489</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="58" t="s">
         <v>490</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="59" t="s">
         <v>491</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="60" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="62" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="62" t="s">
         <v>496</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="63" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="62" t="s">
         <v>498</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="64" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="62" t="s">
         <v>500</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="64" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="7" ht="14.5">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="62" t="s">
         <v>504</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="64" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="8" ht="14.5">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="62" t="s">
         <v>506</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="64" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="9" ht="14.5">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="62" t="s">
         <v>508</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="64" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="10" ht="43.5">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="61" t="s">
         <v>510</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>511</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="63" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>493</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="62" t="s">
         <v>513</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="64" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="D12" s="67"/>
+      <c r="D12" s="66"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="D13" s="67"/>
+      <c r="D13" s="66"/>
     </row>
     <row r="14" ht="14.25" customHeight="1"/>
     <row r="15" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Ricompilazione casi segnalati via mail
Ricompilate colonne da P a S per i casi di test con ID [28, 29, 31, 32, 35, 36, 37, 39, 40, 43, 44, 45, 47, 48, 51, 423, 424, 425] come segnalato da mail ricevuta da fse-pnrr@innovazione.gov.it
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#PIAFONDAZIONEPANICOXX/AZ-PANICO/FSE-PANICO/1.0/report-checklist.xlsx
@@ -346,7 +346,7 @@
     <t xml:space="preserve">Si è verificato un errore durante la comunicazione con FSE. Dettaglio Errore: "Campo token JWT non valido. - Il campo purpose_of_use non è valorizzato". Contattare il CED.</t>
   </si>
   <si>
-    <t xml:space="preserve">Errore segnalato all'utente.</t>
+    <t xml:space="preserve">Errore segnalato all'utente/medico indicando il mancato invio del referto al FSE. Il sistema segnalerà il mancato invio al personale tecnico/backoffice che interverrà per correggere l'errore che ha portato all'errata compilazione del token JWT fino ad ottenere l'effettivo invio del documento al FSE.</t>
   </si>
   <si>
     <t>KO</t>
@@ -527,7 +527,7 @@
     <t xml:space="preserve">Il servizio FSE non è attualmente disponibile, non è possibile validare e pubblicare il referto sul Fascicolo Elettronico del paziente al momento. Verrà tentato in automatico di pubblicarlo in un momento successivo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene segnalato al medico che il servizio di FSE per validare il referto non è raggiungibile. Viene consentito di consegnare il referto al paziente. Un processo in background ritenterà l'invio in un momento successivo.</t>
+    <t xml:space="preserve">Viene segnalato al medico che il servizio di FSE per validare il referto non è raggiungibile. Viene consentito di consegnare il referto al paziente. Un processo in background ritenterà varie volte l'invio. In caso di persistenza dell'irraggiungibilità del servizio, il sistema segnalerà il mancato invio al backoffice che interverrà manualmente per effettuare l'invio quando il sistema tornerà raggiungibile.</t>
   </si>
   <si>
     <t>VALIDAZIONE_LDO_TIMEOUT</t>
@@ -2006,7 +2006,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2383,6 +2383,19 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="none"/>
       <bottom style="thin">
         <color auto="1"/>
@@ -2409,7 +2422,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2542,13 +2555,16 @@
     <xf fontId="2" fillId="0" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="29" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="27" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2557,10 +2573,10 @@
     <xf fontId="2" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="3" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="7" fillId="3" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="3" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="3" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="8" fillId="0" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2569,17 +2585,17 @@
     <xf fontId="9" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="30" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="31" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -4614,7 +4630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" ht="128.25">
+    <row r="10" ht="128.25" hidden="1">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4710,7 +4726,7 @@
         <v>61</v>
       </c>
       <c r="R11" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S11" s="39" t="s">
         <v>63</v>
@@ -4771,7 +4787,7 @@
         <v>61</v>
       </c>
       <c r="R12" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S12" s="39" t="s">
         <v>63</v>
@@ -4869,7 +4885,7 @@
         <v>61</v>
       </c>
       <c r="R14" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S14" s="39" t="s">
         <v>63</v>
@@ -4930,7 +4946,7 @@
         <v>61</v>
       </c>
       <c r="R15" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S15" s="39" t="s">
         <v>63</v>
@@ -5065,7 +5081,7 @@
         <v>61</v>
       </c>
       <c r="R18" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S18" s="39" t="s">
         <v>63</v>
@@ -5126,7 +5142,7 @@
         <v>61</v>
       </c>
       <c r="R19" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S19" s="39" t="s">
         <v>63</v>
@@ -5187,7 +5203,7 @@
         <v>61</v>
       </c>
       <c r="R20" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S20" s="39" t="s">
         <v>63</v>
@@ -5285,7 +5301,7 @@
         <v>61</v>
       </c>
       <c r="R22" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S22" s="39" t="s">
         <v>63</v>
@@ -5346,7 +5362,7 @@
         <v>61</v>
       </c>
       <c r="R23" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S23" s="39" t="s">
         <v>63</v>
@@ -5481,7 +5497,7 @@
         <v>61</v>
       </c>
       <c r="R26" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S26" s="39" t="s">
         <v>63</v>
@@ -5529,16 +5545,16 @@
       <c r="O27" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="P27" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q27" s="51" t="s">
+      <c r="P27" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="S27" s="52" t="s">
+      <c r="Q27" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="R27" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="S27" s="53" t="s">
         <v>110</v>
       </c>
       <c r="T27" s="39"/>
@@ -5577,25 +5593,25 @@
       </c>
       <c r="K28" s="39"/>
       <c r="L28" s="50"/>
-      <c r="M28" s="53" t="s">
+      <c r="M28" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="N28" s="53" t="s">
+      <c r="N28" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="O28" s="53" t="s">
+      <c r="O28" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="P28" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q28" s="53" t="s">
+      <c r="P28" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="R28" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="S28" s="54" t="s">
+      <c r="Q28" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="R28" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="S28" s="55" t="s">
         <v>110</v>
       </c>
       <c r="T28" s="39"/>
@@ -5630,13 +5646,13 @@
       <c r="J29" s="39"/>
       <c r="K29" s="39"/>
       <c r="L29" s="39"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
       <c r="T29" s="39"/>
       <c r="U29" s="40" t="s">
         <v>54</v>
@@ -5682,16 +5698,16 @@
       <c r="O30" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="P30" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q30" s="51" t="s">
+      <c r="P30" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="R30" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="S30" s="52" t="s">
+      <c r="Q30" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="R30" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="S30" s="53" t="s">
         <v>110</v>
       </c>
       <c r="T30" s="39"/>
@@ -5730,28 +5746,28 @@
       </c>
       <c r="K31" s="39"/>
       <c r="L31" s="50"/>
-      <c r="M31" s="53" t="s">
+      <c r="M31" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="N31" s="53" t="s">
+      <c r="N31" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="O31" s="53" t="s">
+      <c r="O31" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="P31" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q31" s="53" t="s">
+      <c r="P31" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="R31" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="S31" s="54" t="s">
+      <c r="Q31" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="R31" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="S31" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="T31" s="56"/>
+      <c r="T31" s="57"/>
       <c r="U31" s="40" t="s">
         <v>54</v>
       </c>
@@ -5783,13 +5799,13 @@
       <c r="J32" s="39"/>
       <c r="K32" s="39"/>
       <c r="L32" s="39"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="56"/>
       <c r="T32" s="39"/>
       <c r="U32" s="40" t="s">
         <v>54</v>
@@ -5875,15 +5891,15 @@
         <v>109</v>
       </c>
       <c r="P34" s="51" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="Q34" s="51" t="s">
         <v>54</v>
       </c>
       <c r="R34" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="S34" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="S34" s="55" t="s">
         <v>110</v>
       </c>
       <c r="T34" s="39"/>
@@ -5895,7 +5911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" ht="39" customHeight="1">
+    <row r="35" ht="39" hidden="1" customHeight="1">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5922,13 +5938,13 @@
         <v>120</v>
       </c>
       <c r="L35" s="39"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
       <c r="T35" s="39"/>
       <c r="U35" s="40"/>
       <c r="V35" s="41"/>
@@ -5936,7 +5952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" ht="39" customHeight="1">
+    <row r="36" ht="39" hidden="1" customHeight="1">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5977,7 +5993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" ht="39" customHeight="1">
+    <row r="37" ht="39" hidden="1" customHeight="1">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -6018,7 +6034,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" ht="39" customHeight="1">
+    <row r="38" ht="39" hidden="1" customHeight="1">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -6059,7 +6075,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" ht="39" customHeight="1">
+    <row r="39" ht="39" hidden="1" customHeight="1">
       <c r="A39" s="35">
         <v>59</v>
       </c>
@@ -6100,7 +6116,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" ht="39" customHeight="1">
+    <row r="40" ht="39" hidden="1" customHeight="1">
       <c r="A40" s="35">
         <v>60</v>
       </c>
@@ -6141,7 +6157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" ht="39" customHeight="1">
+    <row r="41" ht="39" hidden="1" customHeight="1">
       <c r="A41" s="35">
         <v>61</v>
       </c>
@@ -6182,7 +6198,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" ht="39" customHeight="1">
+    <row r="42" ht="39" hidden="1" customHeight="1">
       <c r="A42" s="35">
         <v>62</v>
       </c>
@@ -6223,7 +6239,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" ht="39" customHeight="1">
+    <row r="43" ht="39" hidden="1" customHeight="1">
       <c r="A43" s="35">
         <v>64</v>
       </c>
@@ -6264,7 +6280,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" ht="39" customHeight="1">
+    <row r="44" ht="39" hidden="1" customHeight="1">
       <c r="A44" s="35">
         <v>66</v>
       </c>
@@ -6305,7 +6321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" ht="39" customHeight="1">
+    <row r="45" ht="39" hidden="1" customHeight="1">
       <c r="A45" s="35">
         <v>67</v>
       </c>
@@ -6346,7 +6362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" ht="39" customHeight="1">
+    <row r="46" ht="39" hidden="1" customHeight="1">
       <c r="A46" s="35">
         <v>68</v>
       </c>
@@ -6387,7 +6403,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" ht="39" customHeight="1">
+    <row r="47" ht="39" hidden="1" customHeight="1">
       <c r="A47" s="35">
         <v>69</v>
       </c>
@@ -6428,7 +6444,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" ht="39" customHeight="1">
+    <row r="48" ht="39" hidden="1" customHeight="1">
       <c r="A48" s="35">
         <v>70</v>
       </c>
@@ -6469,7 +6485,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" ht="39" customHeight="1">
+    <row r="49" ht="39" hidden="1" customHeight="1">
       <c r="A49" s="35">
         <v>71</v>
       </c>
@@ -6510,7 +6526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" ht="39" customHeight="1">
+    <row r="50" ht="39" hidden="1" customHeight="1">
       <c r="A50" s="35">
         <v>72</v>
       </c>
@@ -6551,7 +6567,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" ht="39" customHeight="1">
+    <row r="51" ht="39" hidden="1" customHeight="1">
       <c r="A51" s="35">
         <v>73</v>
       </c>
@@ -6592,7 +6608,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" ht="39" customHeight="1">
+    <row r="52" ht="39" hidden="1" customHeight="1">
       <c r="A52" s="35">
         <v>74</v>
       </c>
@@ -6633,7 +6649,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" ht="39" customHeight="1">
+    <row r="53" ht="39" hidden="1" customHeight="1">
       <c r="A53" s="35">
         <v>76</v>
       </c>
@@ -6674,7 +6690,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" ht="39" customHeight="1">
+    <row r="54" ht="39" hidden="1" customHeight="1">
       <c r="A54" s="35">
         <v>78</v>
       </c>
@@ -6715,7 +6731,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" ht="39" customHeight="1">
+    <row r="55" ht="39" hidden="1" customHeight="1">
       <c r="A55" s="35">
         <v>79</v>
       </c>
@@ -6756,7 +6772,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" ht="39" customHeight="1">
+    <row r="56" ht="39" hidden="1" customHeight="1">
       <c r="A56" s="35">
         <v>80</v>
       </c>
@@ -6797,7 +6813,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" ht="39" customHeight="1">
+    <row r="57" ht="39" hidden="1" customHeight="1">
       <c r="A57" s="35">
         <v>81</v>
       </c>
@@ -6838,7 +6854,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" ht="39" customHeight="1">
+    <row r="58" ht="39" hidden="1" customHeight="1">
       <c r="A58" s="35">
         <v>83</v>
       </c>
@@ -6879,7 +6895,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" ht="39" customHeight="1">
+    <row r="59" ht="39" hidden="1" customHeight="1">
       <c r="A59" s="35">
         <v>84</v>
       </c>
@@ -6920,7 +6936,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" ht="39" customHeight="1">
+    <row r="60" ht="39" hidden="1" customHeight="1">
       <c r="A60" s="35">
         <v>85</v>
       </c>
@@ -6961,7 +6977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" ht="39" customHeight="1">
+    <row r="61" ht="39" hidden="1" customHeight="1">
       <c r="A61" s="35">
         <v>86</v>
       </c>
@@ -7002,7 +7018,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" ht="39" customHeight="1">
+    <row r="62" ht="39" hidden="1" customHeight="1">
       <c r="A62" s="35">
         <v>87</v>
       </c>
@@ -7043,7 +7059,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" ht="39" customHeight="1">
+    <row r="63" ht="39" hidden="1" customHeight="1">
       <c r="A63" s="35">
         <v>88</v>
       </c>
@@ -7084,7 +7100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" ht="39" customHeight="1">
+    <row r="64" ht="39" hidden="1" customHeight="1">
       <c r="A64" s="35">
         <v>89</v>
       </c>
@@ -7125,7 +7141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" ht="39" customHeight="1">
+    <row r="65" ht="39" hidden="1" customHeight="1">
       <c r="A65" s="35">
         <v>90</v>
       </c>
@@ -7166,7 +7182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" ht="39" customHeight="1">
+    <row r="66" ht="39" hidden="1" customHeight="1">
       <c r="A66" s="35">
         <v>91</v>
       </c>
@@ -7207,7 +7223,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" ht="39" customHeight="1">
+    <row r="67" ht="39" hidden="1" customHeight="1">
       <c r="A67" s="35">
         <v>92</v>
       </c>
@@ -7248,7 +7264,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" ht="39" customHeight="1">
+    <row r="68" ht="39" hidden="1" customHeight="1">
       <c r="A68" s="35">
         <v>93</v>
       </c>
@@ -8177,7 +8193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="93" ht="39" customHeight="1">
+    <row r="93" ht="39" hidden="1" customHeight="1">
       <c r="A93" s="35">
         <v>123</v>
       </c>
@@ -8218,7 +8234,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" ht="39" customHeight="1">
+    <row r="94" ht="39" hidden="1" customHeight="1">
       <c r="A94" s="35">
         <v>125</v>
       </c>
@@ -8259,7 +8275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" ht="39" customHeight="1">
+    <row r="95" ht="39" hidden="1" customHeight="1">
       <c r="A95" s="35">
         <v>126</v>
       </c>
@@ -8300,7 +8316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" ht="39" customHeight="1">
+    <row r="96" ht="39" hidden="1" customHeight="1">
       <c r="A96" s="35">
         <v>127</v>
       </c>
@@ -8341,7 +8357,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" ht="39" customHeight="1">
+    <row r="97" ht="39" hidden="1" customHeight="1">
       <c r="A97" s="35">
         <v>128</v>
       </c>
@@ -8382,7 +8398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="98" ht="39" customHeight="1">
+    <row r="98" ht="39" hidden="1" customHeight="1">
       <c r="A98" s="35">
         <v>129</v>
       </c>
@@ -8423,7 +8439,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="99" ht="39" customHeight="1">
+    <row r="99" ht="39" hidden="1" customHeight="1">
       <c r="A99" s="35">
         <v>130</v>
       </c>
@@ -8464,7 +8480,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" ht="39" customHeight="1">
+    <row r="100" ht="39" hidden="1" customHeight="1">
       <c r="A100" s="35">
         <v>131</v>
       </c>
@@ -8505,7 +8521,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" ht="39" customHeight="1">
+    <row r="101" ht="39" hidden="1" customHeight="1">
       <c r="A101" s="35">
         <v>132</v>
       </c>
@@ -8546,7 +8562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" ht="39" customHeight="1">
+    <row r="102" ht="39" hidden="1" customHeight="1">
       <c r="A102" s="35">
         <v>133</v>
       </c>
@@ -8587,7 +8603,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="103" ht="39" customHeight="1">
+    <row r="103" ht="39" hidden="1" customHeight="1">
       <c r="A103" s="35">
         <v>134</v>
       </c>
@@ -8628,7 +8644,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="104" ht="39" customHeight="1">
+    <row r="104" ht="39" hidden="1" customHeight="1">
       <c r="A104" s="35">
         <v>135</v>
       </c>
@@ -8669,7 +8685,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="105" ht="39" customHeight="1">
+    <row r="105" ht="39" hidden="1" customHeight="1">
       <c r="A105" s="35">
         <v>136</v>
       </c>
@@ -8710,7 +8726,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="106" ht="39" customHeight="1">
+    <row r="106" ht="39" hidden="1" customHeight="1">
       <c r="A106" s="35">
         <v>137</v>
       </c>
@@ -8751,7 +8767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" ht="39" customHeight="1">
+    <row r="107" ht="39" hidden="1" customHeight="1">
       <c r="A107" s="35">
         <v>138</v>
       </c>
@@ -8792,7 +8808,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="108" ht="39" customHeight="1">
+    <row r="108" ht="39" hidden="1" customHeight="1">
       <c r="A108" s="35">
         <v>139</v>
       </c>
@@ -8833,7 +8849,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="109" ht="39" customHeight="1">
+    <row r="109" ht="39" hidden="1" customHeight="1">
       <c r="A109" s="35">
         <v>140</v>
       </c>
@@ -8874,7 +8890,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" ht="39" customHeight="1">
+    <row r="110" ht="39" hidden="1" customHeight="1">
       <c r="A110" s="35">
         <v>141</v>
       </c>
@@ -8915,7 +8931,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="111" ht="39" customHeight="1">
+    <row r="111" ht="39" hidden="1" customHeight="1">
       <c r="A111" s="35">
         <v>142</v>
       </c>
@@ -8956,7 +8972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="112" ht="39" customHeight="1">
+    <row r="112" ht="39" hidden="1" customHeight="1">
       <c r="A112" s="35">
         <v>143</v>
       </c>
@@ -8997,7 +9013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="113" ht="39" customHeight="1">
+    <row r="113" ht="39" hidden="1" customHeight="1">
       <c r="A113" s="35">
         <v>144</v>
       </c>
@@ -9038,7 +9054,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="114" ht="39" customHeight="1">
+    <row r="114" ht="39" hidden="1" customHeight="1">
       <c r="A114" s="35">
         <v>145</v>
       </c>
@@ -9079,7 +9095,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="115" ht="39" customHeight="1">
+    <row r="115" ht="39" hidden="1" customHeight="1">
       <c r="A115" s="35">
         <v>146</v>
       </c>
@@ -9120,7 +9136,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="116" ht="78" customHeight="1">
+    <row r="116" ht="78" hidden="1" customHeight="1">
       <c r="A116" s="35">
         <v>152</v>
       </c>
@@ -9161,7 +9177,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="117" ht="39" customHeight="1">
+    <row r="117" ht="39" hidden="1" customHeight="1">
       <c r="A117" s="35">
         <v>154</v>
       </c>
@@ -9202,7 +9218,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="118" ht="39" customHeight="1">
+    <row r="118" ht="39" hidden="1" customHeight="1">
       <c r="A118" s="35">
         <v>155</v>
       </c>
@@ -9243,7 +9259,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" ht="39" customHeight="1">
+    <row r="119" ht="39" hidden="1" customHeight="1">
       <c r="A119" s="35">
         <v>156</v>
       </c>
@@ -9284,7 +9300,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="120" ht="39" customHeight="1">
+    <row r="120" ht="39" hidden="1" customHeight="1">
       <c r="A120" s="35">
         <v>159</v>
       </c>
@@ -9325,7 +9341,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="121" ht="39" customHeight="1">
+    <row r="121" ht="39" hidden="1" customHeight="1">
       <c r="A121" s="35">
         <v>160</v>
       </c>
@@ -9366,7 +9382,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="122" ht="39" customHeight="1">
+    <row r="122" ht="39" hidden="1" customHeight="1">
       <c r="A122" s="35">
         <v>161</v>
       </c>
@@ -9407,7 +9423,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="123" ht="39" customHeight="1">
+    <row r="123" ht="39" hidden="1" customHeight="1">
       <c r="A123" s="35">
         <v>162</v>
       </c>
@@ -9448,7 +9464,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="124" ht="39" customHeight="1">
+    <row r="124" ht="39" hidden="1" customHeight="1">
       <c r="A124" s="35">
         <v>163</v>
       </c>
@@ -9489,7 +9505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" ht="39" customHeight="1">
+    <row r="125" ht="39" hidden="1" customHeight="1">
       <c r="A125" s="35">
         <v>164</v>
       </c>
@@ -9530,7 +9546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="126" ht="39" customHeight="1">
+    <row r="126" ht="39" hidden="1" customHeight="1">
       <c r="A126" s="35">
         <v>165</v>
       </c>
@@ -9571,7 +9587,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" ht="39" customHeight="1">
+    <row r="127" ht="39" hidden="1" customHeight="1">
       <c r="A127" s="35">
         <v>166</v>
       </c>
@@ -9612,7 +9628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="128" ht="39" customHeight="1">
+    <row r="128" ht="39" hidden="1" customHeight="1">
       <c r="A128" s="35">
         <v>167</v>
       </c>
@@ -9653,7 +9669,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" ht="39" customHeight="1">
+    <row r="129" ht="39" hidden="1" customHeight="1">
       <c r="A129" s="35">
         <v>168</v>
       </c>
@@ -9694,7 +9710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="130" ht="39" customHeight="1">
+    <row r="130" ht="39" hidden="1" customHeight="1">
       <c r="A130" s="35">
         <v>169</v>
       </c>
@@ -10290,7 +10306,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" ht="15">
+    <row r="146" ht="15" hidden="1">
       <c r="A146" s="35">
         <v>191</v>
       </c>
@@ -10337,7 +10353,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="147" ht="39" customHeight="1">
+    <row r="147" ht="39" hidden="1" customHeight="1">
       <c r="A147" s="35">
         <v>376</v>
       </c>
@@ -10380,7 +10396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="148" ht="39" customHeight="1">
+    <row r="148" ht="39" hidden="1" customHeight="1">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -10427,7 +10443,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="149" ht="39" customHeight="1">
+    <row r="149" ht="39" hidden="1" customHeight="1">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -10474,7 +10490,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="150" ht="39" customHeight="1">
+    <row r="150" ht="39" hidden="1" customHeight="1">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -10570,7 +10586,7 @@
         <v>61</v>
       </c>
       <c r="R151" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S151" s="39" t="s">
         <v>63</v>
@@ -10631,7 +10647,7 @@
         <v>61</v>
       </c>
       <c r="R152" s="39" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="S152" s="39" t="s">
         <v>63</v>
@@ -10680,15 +10696,15 @@
         <v>109</v>
       </c>
       <c r="P153" s="51" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="Q153" s="51" t="s">
         <v>54</v>
       </c>
       <c r="R153" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="S153" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="S153" s="55" t="s">
         <v>110</v>
       </c>
       <c r="T153" s="39"/>
@@ -10700,7 +10716,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="154" ht="39" customHeight="1">
+    <row r="154" ht="39" hidden="1" customHeight="1">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -10727,13 +10743,13 @@
         <v>120</v>
       </c>
       <c r="L154" s="39"/>
-      <c r="M154" s="55"/>
-      <c r="N154" s="55"/>
-      <c r="O154" s="55"/>
-      <c r="P154" s="55"/>
-      <c r="Q154" s="55"/>
-      <c r="R154" s="55"/>
-      <c r="S154" s="55"/>
+      <c r="M154" s="56"/>
+      <c r="N154" s="56"/>
+      <c r="O154" s="56"/>
+      <c r="P154" s="56"/>
+      <c r="Q154" s="56"/>
+      <c r="R154" s="56"/>
+      <c r="S154" s="56"/>
       <c r="T154" s="39"/>
       <c r="U154" s="40"/>
       <c r="V154" s="41"/>
@@ -10741,7 +10757,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="155" ht="39" customHeight="1">
+    <row r="155" ht="39" hidden="1" customHeight="1">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -10782,7 +10798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="156" ht="39" customHeight="1">
+    <row r="156" ht="39" hidden="1" customHeight="1">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -10823,7 +10839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" ht="39" customHeight="1">
+    <row r="157" ht="39" hidden="1" customHeight="1">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -10864,7 +10880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="158" ht="39" customHeight="1">
+    <row r="158" ht="39" hidden="1" customHeight="1">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -10905,7 +10921,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="159" ht="39" customHeight="1">
+    <row r="159" ht="39" hidden="1" customHeight="1">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -10946,7 +10962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="160" ht="39" customHeight="1">
+    <row r="160" ht="39" hidden="1" customHeight="1">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -10987,7 +11003,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="161" ht="39" customHeight="1">
+    <row r="161" ht="39" hidden="1" customHeight="1">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -11028,7 +11044,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="162" ht="39" customHeight="1">
+    <row r="162" ht="39" hidden="1" customHeight="1">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -11069,7 +11085,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" ht="39" customHeight="1">
+    <row r="163" ht="39" hidden="1" customHeight="1">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -11184,7 +11200,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="166" ht="39" customHeight="1">
+    <row r="166" ht="39" hidden="1" customHeight="1">
       <c r="A166" s="35">
         <v>448</v>
       </c>
@@ -11231,7 +11247,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="167" ht="33" customHeight="1">
+    <row r="167" ht="33" hidden="1" customHeight="1">
       <c r="A167" s="35">
         <v>449</v>
       </c>
@@ -11278,7 +11294,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="168" ht="33.75" customHeight="1">
+    <row r="168" ht="33.75" hidden="1" customHeight="1">
       <c r="A168" s="35">
         <v>450</v>
       </c>
@@ -11325,7 +11341,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="169" ht="20.25" customHeight="1">
+    <row r="169" ht="20.25" hidden="1" customHeight="1">
       <c r="A169" s="35">
         <v>451</v>
       </c>
@@ -11372,7 +11388,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="170" ht="15">
+    <row r="170" ht="15" hidden="1">
       <c r="A170" s="35">
         <v>452</v>
       </c>
@@ -11419,7 +11435,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" ht="14.25" customHeight="1">
+    <row r="171" ht="14.25" hidden="1" customHeight="1">
       <c r="A171" s="35">
         <v>454</v>
       </c>
@@ -11466,7 +11482,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="172" ht="14.25" customHeight="1">
+    <row r="172" ht="14.25" hidden="1" customHeight="1">
       <c r="A172" s="35">
         <v>455</v>
       </c>
@@ -11661,7 +11677,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="177" ht="15">
+    <row r="177" ht="15" hidden="1">
       <c r="A177" s="35">
         <v>460</v>
       </c>
@@ -11708,7 +11724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="178" ht="14.25" customHeight="1">
+    <row r="178" ht="14.25" hidden="1" customHeight="1">
       <c r="A178" s="35">
         <v>461</v>
       </c>
@@ -11749,7 +11765,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="179" ht="15">
+    <row r="179" ht="15" hidden="1">
       <c r="A179" s="35">
         <v>462</v>
       </c>
@@ -11790,7 +11806,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="180" ht="14.25" customHeight="1">
+    <row r="180" ht="14.25" hidden="1" customHeight="1">
       <c r="A180" s="35">
         <v>463</v>
       </c>
@@ -11905,7 +11921,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" ht="15">
+    <row r="183" ht="15" hidden="1">
       <c r="A183" s="35">
         <v>466</v>
       </c>
@@ -11946,7 +11962,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="184" ht="14.25" customHeight="1">
+    <row r="184" ht="14.25" hidden="1" customHeight="1">
       <c r="A184" s="35">
         <v>467</v>
       </c>
@@ -11987,7 +12003,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="185" ht="22.5" customHeight="1">
+    <row r="185" ht="22.5" hidden="1" customHeight="1">
       <c r="A185" s="35">
         <v>468</v>
       </c>
@@ -12065,7 +12081,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="187" ht="15">
+    <row r="187" ht="15" hidden="1">
       <c r="A187" s="35">
         <v>470</v>
       </c>
@@ -12106,7 +12122,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="188" ht="15">
+    <row r="188" ht="15" hidden="1">
       <c r="A188" s="35">
         <v>471</v>
       </c>
@@ -12153,7 +12169,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="189" ht="15">
+    <row r="189" ht="15" hidden="1">
       <c r="A189" s="35">
         <v>472</v>
       </c>
@@ -12200,7 +12216,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="190" ht="15">
+    <row r="190" ht="15" hidden="1">
       <c r="A190" s="35">
         <v>473</v>
       </c>
@@ -12241,7 +12257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="191" ht="15">
+    <row r="191" ht="15" hidden="1">
       <c r="A191" s="35">
         <v>474</v>
       </c>
@@ -12282,7 +12298,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="192" ht="29.25" customHeight="1">
+    <row r="192" ht="29.25" hidden="1" customHeight="1">
       <c r="A192" s="35">
         <v>475</v>
       </c>
@@ -16351,6 +16367,28 @@
         <filter val="VPS"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="28"/>
+        <filter val="29"/>
+        <filter val="31"/>
+        <filter val="32"/>
+        <filter val="35"/>
+        <filter val="36"/>
+        <filter val="37"/>
+        <filter val="39"/>
+        <filter val="40"/>
+        <filter val="43"/>
+        <filter val="44"/>
+        <filter val="45"/>
+        <filter val="47"/>
+        <filter val="48"/>
+        <filter val="51"/>
+        <filter val="423"/>
+        <filter val="424"/>
+        <filter val="425"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
@@ -16361,8 +16399,8 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <dataValidations count="97" disablePrompts="0">
-    <dataValidation sqref="P10:R10 P13:R13 P15:R17 P21:R21 P24:R25 P29:R29 P32:R33 P35:R150 P154:R192 J10:J11 J13:J17 J21:J22 J24:J25 J29 J31:J33 J69:J92 J116 J118:J121 J131:J148 J164:J165 J168 J170:J177 J180:J182 J186 J188:J189 M10:N10 M13:N17 M21:N21 M24:N25 M29:N29 M32:N33 M35:N150 M154:N192" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+  <dataValidations count="114" disablePrompts="0">
+    <dataValidation sqref="P10:R10 P13:R13 P16:R17 P21:R21 P24:R25 P29:R29 P32:R33 P35:R150 P154:R192 J10:J11 J13:J17 J21:J22 J24:J25 J29 J31:J33 J69:J92 J116 J118:J121 J131:J148 J164:J165 J168 J170:J177 J180:J182 J186 J188:J189 M10:N10 M13:N17 M21:N21 M24:N25 M29:N29 M32:N33 M35:N150 M154:N192" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="T10:T152 T154:T192" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
@@ -16375,9 +16413,6 @@
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="M23:N23" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="P23:R23" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="J117" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
@@ -16425,19 +16460,10 @@
     <dataValidation sqref="M20:N20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="P18:R18" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="P20:R20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
     <dataValidation sqref="J12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="M12:N12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="P12:R12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="J20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
@@ -16447,9 +16473,6 @@
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="M26:N26" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="P26:R26" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="J28" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
@@ -16548,15 +16571,6 @@
     <dataValidation sqref="M19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="P19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="Q19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="R19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-      <formula1>Sheet1!$B$2:$B$3</formula1>
-    </dataValidation>
     <dataValidation sqref="J27" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
@@ -16617,6 +16631,27 @@
     <dataValidation sqref="J153" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
+    <dataValidation sqref="N22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="M22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="M151:N151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="M152:N152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
     <dataValidation sqref="P14" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
@@ -16626,10 +16661,40 @@
     <dataValidation sqref="R14" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="N22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="P15" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="M22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="Q15" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R15" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P18" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q18" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R18" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R19" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R20" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
     <dataValidation sqref="P22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
@@ -16641,16 +16706,40 @@
     <dataValidation sqref="R22" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="M151:N151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="P23" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="P151:R151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="Q23" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="M152:N152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="R23" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="P152:R152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="P26" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q26" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R26" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R151" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="P152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="R152" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -16739,170 +16828,170 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>489</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>490</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="60" t="s">
         <v>491</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="61" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="63" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="64" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="63" t="s">
         <v>496</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="64" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="63" t="s">
         <v>498</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="65" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="63" t="s">
         <v>500</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="64" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="63" t="s">
         <v>502</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="65" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="7" ht="14.5">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="63" t="s">
         <v>504</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="65" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="8" ht="14.5">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="63" t="s">
         <v>506</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="65" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="9" ht="14.5">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="63" t="s">
         <v>508</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="65" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="10" ht="43.5">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="62" t="s">
         <v>510</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="66" t="s">
         <v>511</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="64" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="62" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="62" t="s">
         <v>493</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="63" t="s">
         <v>513</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="65" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="D12" s="66"/>
+      <c r="D12" s="67"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="D13" s="66"/>
+      <c r="D13" s="67"/>
     </row>
     <row r="14" ht="14.25" customHeight="1"/>
     <row r="15" ht="14.25" customHeight="1"/>

</xml_diff>